<commit_message>
validacion de rubros (reverted from commit 169b1b283069fa0795dde074a02930536ea7f9fa)
</commit_message>
<xml_diff>
--- a/Documentos/CAMPOSNUEVOSIB.xlsx
+++ b/Documentos/CAMPOSNUEVOSIB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="5970" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="5970" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="131">
   <si>
     <t xml:space="preserve">TIPO </t>
   </si>
@@ -410,24 +410,6 @@
   </si>
   <si>
     <t>4028E6C72959682B01295F40BC2A02E2</t>
-  </si>
-  <si>
-    <t>i_errormsg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV </t>
-  </si>
-  <si>
-    <t>i_isimported</t>
-  </si>
-  <si>
-    <t>CHARACTER</t>
-  </si>
-  <si>
-    <t>processing</t>
-  </si>
-  <si>
-    <t>processed</t>
   </si>
 </sst>
 </file>
@@ -1617,72 +1599,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C4">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1694,7 +1624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
validacion de rubros (reverted from commit 169b1b283069fa0795dde074a02930536ea7f9fa) (reverted from commit e42486eed160d7668eb1c0e2341e8f7d24b38d86)
</commit_message>
<xml_diff>
--- a/Documentos/CAMPOSNUEVOSIB.xlsx
+++ b/Documentos/CAMPOSNUEVOSIB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="5970" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="5970" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="137">
   <si>
     <t xml:space="preserve">TIPO </t>
   </si>
@@ -410,6 +410,24 @@
   </si>
   <si>
     <t>4028E6C72959682B01295F40BC2A02E2</t>
+  </si>
+  <si>
+    <t>i_errormsg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV </t>
+  </si>
+  <si>
+    <t>i_isimported</t>
+  </si>
+  <si>
+    <t>CHARACTER</t>
+  </si>
+  <si>
+    <t>processing</t>
+  </si>
+  <si>
+    <t>processed</t>
   </si>
 </sst>
 </file>
@@ -1599,20 +1617,72 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1624,7 +1694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>

</xml_diff>